<commit_message>
adds spanish flag words
</commit_message>
<xml_diff>
--- a/process/flag-words.xlsx
+++ b/process/flag-words.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandiehm/Sites/same-sex-songs/process/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348667E7-8028-2A45-894D-33CA928D38AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="47480" yWindow="4520" windowWidth="25600" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="womanFlags" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="manFlags" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="loveFlags" sheetId="3" r:id="rId6"/>
+    <sheet name="womanFlags" sheetId="1" r:id="rId1"/>
+    <sheet name="manFlags" sheetId="2" r:id="rId2"/>
+    <sheet name="loveFlags" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>girl</t>
   </si>
@@ -181,70 +190,100 @@
   </si>
   <si>
     <t>beso</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>ladies</t>
+  </si>
+  <si>
+    <t>esposa</t>
+  </si>
+  <si>
+    <t>prometida</t>
+  </si>
+  <si>
+    <t>chico</t>
+  </si>
+  <si>
+    <t>nina</t>
+  </si>
+  <si>
+    <t>prometido</t>
+  </si>
+  <si>
+    <t>esposo</t>
+  </si>
+  <si>
+    <t>men</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -434,330 +473,386 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more plural flag words, update readme
</commit_message>
<xml_diff>
--- a/process/flag-words.xlsx
+++ b/process/flag-words.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandiehm/Sites/same-sex-songs/process/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelsey\Desktop\Website\Projects\Same-Sex Songs\same-sex-songs\process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912AF60-BD1D-B949-9CBD-BB84AB547710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47480" yWindow="4520" windowWidth="25600" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47475" yWindow="4515" windowWidth="25605" windowHeight="20340"/>
   </bookViews>
   <sheets>
     <sheet name="womanFlags" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>girl</t>
   </si>
@@ -198,18 +197,12 @@
     <t>ladies</t>
   </si>
   <si>
-    <t>esposa</t>
-  </si>
-  <si>
     <t>prometida</t>
   </si>
   <si>
     <t>chico</t>
   </si>
   <si>
-    <t>nina</t>
-  </si>
-  <si>
     <t>prometido</t>
   </si>
   <si>
@@ -219,7 +212,91 @@
     <t>men</t>
   </si>
   <si>
-    <t>senor</t>
+    <t>girls</t>
+  </si>
+  <si>
+    <t>girlfriends</t>
+  </si>
+  <si>
+    <t>females</t>
+  </si>
+  <si>
+    <t>hoes</t>
+  </si>
+  <si>
+    <t>shawties</t>
+  </si>
+  <si>
+    <t>shorties</t>
+  </si>
+  <si>
+    <t>thots</t>
+  </si>
+  <si>
+    <t>chicks</t>
+  </si>
+  <si>
+    <t>ellas</t>
+  </si>
+  <si>
+    <t>novias</t>
+  </si>
+  <si>
+    <t>chicas</t>
+  </si>
+  <si>
+    <t>mujer</t>
+  </si>
+  <si>
+    <t>mujeres</t>
+  </si>
+  <si>
+    <t>señorita</t>
+  </si>
+  <si>
+    <t>señoritas</t>
+  </si>
+  <si>
+    <t>niñas</t>
+  </si>
+  <si>
+    <t>niña</t>
+  </si>
+  <si>
+    <t>boys</t>
+  </si>
+  <si>
+    <t>boyfriends</t>
+  </si>
+  <si>
+    <t>males</t>
+  </si>
+  <si>
+    <t>guys</t>
+  </si>
+  <si>
+    <t>dudes</t>
+  </si>
+  <si>
+    <t>ellos</t>
+  </si>
+  <si>
+    <t>novios</t>
+  </si>
+  <si>
+    <t>chicos</t>
+  </si>
+  <si>
+    <t>niño</t>
+  </si>
+  <si>
+    <t>niños</t>
+  </si>
+  <si>
+    <t>señor</t>
+  </si>
+  <si>
+    <t>señores</t>
   </si>
   <si>
     <t>senorita</t>
@@ -228,7 +305,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -485,141 +562,216 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
+    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
+    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>66</v>
+    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -628,111 +780,166 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>65</v>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -741,129 +948,129 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Extract beg and end phrases too
</commit_message>
<xml_diff>
--- a/process/flag-words.xlsx
+++ b/process/flag-words.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="47475" yWindow="4515" windowWidth="25605" windowHeight="20340"/>
+    <workbookView xWindow="47475" yWindow="4515" windowWidth="25605" windowHeight="20340" tabRatio="726" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="womanFlags" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -320,6 +320,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -341,16 +347,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,7 +576,7 @@
   </sheetPr>
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -954,8 +962,8 @@
   </sheetPr>
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>